<commit_message>
Fix can't configure benchmark on BenchmarkDotNet
</commit_message>
<xml_diff>
--- a/Benchmark/dynamic-result.xlsx
+++ b/Benchmark/dynamic-result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cabdf30199810cd7/home/DynaJson/gitrepo/Benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="807" documentId="8_{9686923D-9FB1-46FC-B3CE-1EAAC94F533E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AFD51334-9F16-447F-986D-444677A44523}"/>
+  <xr:revisionPtr revIDLastSave="869" documentId="8_{9686923D-9FB1-46FC-B3CE-1EAAC94F533E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49F27E1C-361C-4598-ABA4-4485374C3F62}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2400" yWindow="1560" windowWidth="15030" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark.BenchmarkDotNet.Dynam" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,18 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="68" r:id="rId9"/>
-    <pivotCache cacheId="76" r:id="rId10"/>
-    <pivotCache cacheId="79" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2337,7 +2340,7 @@
         <c:idx val="7"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent5"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2397,7 +2400,7 @@
         <c:idx val="8"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent2"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2457,7 +2460,7 @@
         <c:idx val="9"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent3"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2517,7 +2520,7 @@
         <c:idx val="10"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent5"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2674,6 +2677,26 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1206-4EAB-A136-2F4B8F249007}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-1206-4EAB-A136-2F4B8F249007}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -2851,6 +2874,16 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-1206-4EAB-A136-2F4B8F249007}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="4"/>
@@ -3007,6 +3040,16 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1206-4EAB-A136-2F4B8F249007}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -3298,6 +3341,26 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-1206-4EAB-A136-2F4B8F249007}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1206-4EAB-A136-2F4B8F249007}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -4184,7 +4247,7 @@
         <c:idx val="6"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent2"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -4244,7 +4307,7 @@
         <c:idx val="7"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent2"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -4466,6 +4529,26 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-09C3-462A-A98F-644BE33DB619}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-09C3-462A-A98F-644BE33DB619}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -5785,6 +5868,9 @@
           </a:ln>
           <a:effectLst/>
         </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:numFmt formatCode="0_);[Red]\(0\)" sourceLinked="0"/>
@@ -8611,7 +8697,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{14CBB3D1-92F4-4DC6-97D8-54F1ECEEA169}" name="ピボットテーブル1" cacheId="68" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{14CBB3D1-92F4-4DC6-97D8-54F1ECEEA169}" name="ピボットテーブル1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A1:G8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -8860,7 +8946,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E61C71FD-DD2C-4C9D-8A07-729F5EADB217}" name="ピボットテーブル1" cacheId="79" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E61C71FD-DD2C-4C9D-8A07-729F5EADB217}" name="ピボットテーブル1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A1:G8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -9048,7 +9134,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{19C3E097-3CBF-4A33-A5DC-3FEBD6F408AD}" name="ピボットテーブル3" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{19C3E097-3CBF-4A33-A5DC-3FEBD6F408AD}" name="ピボットテーブル3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A1:D8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
@@ -9516,8 +9602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AZ61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -19172,7 +19258,7 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D61"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -21927,7 +22013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAE602A-4F40-4829-B9AD-28C5D9418B07}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>